<commit_message>
Added pitch percent to the data and reran the feature selection
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanyohnk/Dropbox/dev/baseball/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{ACBFAEFD-1A1E-9348-9BBC-EF91397E4102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A73C74-C8D0-C042-AA77-E86FF737CB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36760" yWindow="-2440" windowWidth="28040" windowHeight="17200"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
   <si>
     <t>year</t>
   </si>
@@ -389,12 +389,21 @@
   </si>
   <si>
     <t>Wainwright</t>
+  </si>
+  <si>
+    <t>ERA</t>
+  </si>
+  <si>
+    <t>so - walk</t>
+  </si>
+  <si>
+    <t>pred_so/walk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1228,16 +1237,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1265,8 +1277,17 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -1295,7 +1316,7 @@
         <v>1.4866996417670399</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -1324,7 +1345,7 @@
         <v>0.85336082257554802</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -1353,7 +1374,7 @@
         <v>0.80692074029277905</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -1382,7 +1403,7 @@
         <v>0.56136368173214901</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -1411,7 +1432,7 @@
         <v>0.48105094249086799</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -1440,7 +1461,7 @@
         <v>0.459976114415454</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -1469,7 +1490,7 @@
         <v>0.445704075966529</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -1498,7 +1519,7 @@
         <v>0.39086362398274499</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -1527,7 +1548,7 @@
         <v>0.382300424416464</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -1556,7 +1577,7 @@
         <v>0.379964643542898</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2022</v>
       </c>
@@ -1585,7 +1606,7 @@
         <v>0.35445012888119498</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2022</v>
       </c>
@@ -1614,7 +1635,7 @@
         <v>0.32891967108951498</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -1643,7 +1664,7 @@
         <v>0.29645309719322899</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2022</v>
       </c>
@@ -1672,7 +1693,7 @@
         <v>0.28887521691547802</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2022</v>
       </c>

</xml_diff>